<commit_message>
Final Route GET tags
</commit_message>
<xml_diff>
--- a/lista_etiquetas.xlsx
+++ b/lista_etiquetas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21420" windowHeight="10005" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12495" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -80,10 +80,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -99,6 +99,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -106,9 +113,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -116,30 +137,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -198,53 +198,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,37 +265,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,145 +439,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,17 +459,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -485,15 +479,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,6 +516,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -546,161 +542,165 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1095,10 +1095,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1232,6 +1232,9 @@
       <c r="E9">
         <v>5.6</v>
       </c>
+    </row>
+    <row r="10" spans="4:4">
+      <c r="D10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Final Route PUT tags
</commit_message>
<xml_diff>
--- a/lista_etiquetas.xlsx
+++ b/lista_etiquetas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
@@ -34,12 +34,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="5">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -403,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -438,16 +434,16 @@
         <v>AA123456789BR</v>
       </c>
       <c r="B4" t="str">
-        <v>Fulano da Silva 1</v>
+        <v>Fulano Sousa 1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>39645000</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
@@ -501,10 +497,44 @@
         <v>399</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>AE123456789BR</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Fulano da Silva 5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>13610720</v>
+      </c>
+      <c r="E8">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>AF123456789BR</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Fulano da Silva 6</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>19050280</v>
+      </c>
+      <c r="E9">
+        <v>5.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E9"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>